<commit_message>
Modified EmployeeCreateTestPage to read data from Excel
</commit_message>
<xml_diff>
--- a/src/main/java/com/jala/qa/DataLayer/mybook.xlsx
+++ b/src/main/java/com/jala/qa/DataLayer/mybook.xlsx
@@ -5,15 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenovo\eclipse-workspace\Automation_project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/afe5129fceb5a64b/Desktop/project/Selenium_Java_Project_Batch_Nov2025_9PM/src/main/java/com/jala/qa/DataLayer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AEE7C3E-986F-405E-B90A-D87B0B412A8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="13_ncr:1_{2AEE7C3E-986F-405E-B90A-D87B0B412A8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EFE82D1F-183C-4901-BB0D-232138C6240C}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="EmployeeData" sheetId="3" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -26,97 +26,202 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="28">
-  <si>
-    <t>--Select Country--</t>
-  </si>
-  <si>
-    <t>Bangladesh</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="63">
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>TC id</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>expected result</t>
+  </si>
+  <si>
+    <t>Actual result</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>https://magnus.jalatechnologies.com/Home/Index</t>
+  </si>
+  <si>
+    <t>training@jalaacademy.com</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>Demo</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>jobprogram</t>
+  </si>
+  <si>
+    <t>admin123</t>
+  </si>
+  <si>
+    <t>xyz</t>
+  </si>
+  <si>
+    <t>https://magnus.jalatechnologies.com/</t>
+  </si>
+  <si>
+    <t>failed</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Mobile</t>
+  </si>
+  <si>
+    <t>DOB</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Skill</t>
+  </si>
+  <si>
+    <t>Sheetal</t>
+  </si>
+  <si>
+    <t>Raibole</t>
+  </si>
+  <si>
+    <t>sheetal@test.com</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Koregaon Park 411014</t>
+  </si>
+  <si>
+    <t>Pune</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Doe</t>
+  </si>
+  <si>
+    <t>john.doe@work.com</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>123 Main St, New York</t>
+  </si>
+  <si>
+    <t>Riya</t>
+  </si>
+  <si>
+    <t>Sharma</t>
+  </si>
+  <si>
+    <t>riya.s@corp.com</t>
+  </si>
+  <si>
+    <t>456 Tech Lane, Bangalore</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>Lee</t>
+  </si>
+  <si>
+    <t>david.lee@newco.net</t>
+  </si>
+  <si>
+    <t>10 Downing Street, London</t>
+  </si>
+  <si>
+    <t>Priya</t>
+  </si>
+  <si>
+    <t>Joshi</t>
+  </si>
+  <si>
+    <t>priya.j@devteam.org</t>
+  </si>
+  <si>
+    <t>Cyber Towers, Hitech City</t>
+  </si>
+  <si>
+    <t>Hyderabad</t>
+  </si>
+  <si>
+    <t>Full Stack Developer</t>
+  </si>
+  <si>
+    <t>DevOps</t>
+  </si>
+  <si>
+    <t>Middleware</t>
+  </si>
+  <si>
+    <t>AWS</t>
+  </si>
+  <si>
+    <t>WebServices</t>
+  </si>
+  <si>
+    <t>Sri Lanka</t>
+  </si>
+  <si>
+    <t>Japan</t>
+  </si>
+  <si>
+    <t>Yamagata</t>
+  </si>
+  <si>
+    <t>Dambulla</t>
   </si>
   <si>
     <t>Canada</t>
   </si>
   <si>
-    <t>China</t>
-  </si>
-  <si>
-    <t>France</t>
-  </si>
-  <si>
-    <t>India</t>
-  </si>
-  <si>
-    <t>Japan</t>
-  </si>
-  <si>
-    <t>Nepal</t>
-  </si>
-  <si>
-    <t>Sri Lanka</t>
-  </si>
-  <si>
-    <t>UK</t>
-  </si>
-  <si>
-    <t>USA</t>
-  </si>
-  <si>
-    <t>TC id</t>
-  </si>
-  <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>expected result</t>
-  </si>
-  <si>
-    <t>Actual result</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>https://magnus.jalatechnologies.com/Home/Index</t>
-  </si>
-  <si>
-    <t>training@jalaacademy.com</t>
-  </si>
-  <si>
-    <t>Admin</t>
-  </si>
-  <si>
-    <t>Demo</t>
-  </si>
-  <si>
-    <t>abc</t>
-  </si>
-  <si>
-    <t>jobprogram</t>
-  </si>
-  <si>
-    <t>admin123</t>
-  </si>
-  <si>
-    <t>xyz</t>
-  </si>
-  <si>
-    <t>https://magnus.jalatechnologies.com/</t>
-  </si>
-  <si>
-    <t>failed</t>
-  </si>
-  <si>
-    <t>Pass</t>
+    <t>Cornwall</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,6 +242,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Source Sans Pro"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -180,7 +291,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -191,6 +302,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -470,73 +585,213 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="E1:E11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A151CA25-CF78-4BD5-A3BA-AA2C5D81F3B5}">
+  <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="21.81640625" customWidth="1"/>
-    <col min="4" max="4" width="29.1796875" customWidth="1"/>
-    <col min="5" max="5" width="15.08984375" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" customWidth="1"/>
+    <col min="4" max="4" width="25.88671875" customWidth="1"/>
+    <col min="5" max="5" width="19.21875" customWidth="1"/>
+    <col min="7" max="7" width="22.5546875" customWidth="1"/>
+    <col min="9" max="9" width="15.5546875" customWidth="1"/>
+    <col min="10" max="10" width="18.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="4">
+        <v>9876543210</v>
+      </c>
+      <c r="E2" s="5">
+        <v>35706</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E11" t="s">
-        <v>10</v>
+      <c r="I2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="4">
+        <v>9123456780</v>
+      </c>
+      <c r="E3" s="5">
+        <v>31187</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="4">
+        <v>8887776660</v>
+      </c>
+      <c r="E4" s="5">
+        <v>35034</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="4">
+        <v>7001234567</v>
+      </c>
+      <c r="E5" s="5">
+        <v>33100</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="4">
+        <v>8554443332</v>
+      </c>
+      <c r="E6" s="5">
+        <v>34084</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -548,158 +803,158 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91328408-809F-4054-A405-B3B736A44BED}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
-    <col min="2" max="2" width="44.90625" customWidth="1"/>
-    <col min="3" max="3" width="12.453125" customWidth="1"/>
-    <col min="4" max="4" width="55.453125" customWidth="1"/>
-    <col min="5" max="5" width="36.1796875" customWidth="1"/>
-    <col min="6" max="6" width="17.26953125" customWidth="1"/>
+    <col min="2" max="2" width="44.88671875" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" customWidth="1"/>
+    <col min="4" max="4" width="55.44140625" customWidth="1"/>
+    <col min="5" max="5" width="36.21875" customWidth="1"/>
+    <col min="6" max="6" width="17.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="F2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="37" x14ac:dyDescent="0.45">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="F4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="37" x14ac:dyDescent="0.45">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="36" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" t="s">
         <v>17</v>
       </c>
-      <c r="E5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="6" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="F6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="37" x14ac:dyDescent="0.45">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="36" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" t="s">
         <v>17</v>
-      </c>
-      <c r="E7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>